<commit_message>
MAke entry in the database for new products and masks
</commit_message>
<xml_diff>
--- a/static/add_products_template.xlsx
+++ b/static/add_products_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leharbhatt/P9_New_Product_Customizor_App/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B728A0DE-9262-0E45-A22D-B555C44E4B62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF403CA5-CFDE-9E4F-9457-FBEEC8B4F2C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F36F7B3E-06A3-9447-9F11-6C3B77302C92}"/>
   </bookViews>
@@ -32,15 +32,80 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+  <si>
+    <t>product_title</t>
+  </si>
+  <si>
+    <t>product_description</t>
+  </si>
+  <si>
+    <t>product_price</t>
+  </si>
+  <si>
+    <t>product_category</t>
+  </si>
+  <si>
+    <t>customizable</t>
+  </si>
+  <si>
+    <t>product_image</t>
+  </si>
+  <si>
+    <t>occasion</t>
+  </si>
+  <si>
+    <t>modal_mask</t>
+  </si>
+  <si>
+    <t>text_mask</t>
+  </si>
+  <si>
+    <t>Placard</t>
+  </si>
+  <si>
+    <t>Christmas</t>
+  </si>
+  <si>
+    <t>TestProduct2</t>
+  </si>
+  <si>
+    <t>TestProduct3</t>
+  </si>
+  <si>
+    <t>TestProduct1</t>
+  </si>
+  <si>
+    <t>testing1</t>
+  </si>
+  <si>
+    <t>testing2</t>
+  </si>
+  <si>
+    <t>testing3</t>
+  </si>
+  <si>
+    <t>/Users/leharbhatt/Desktop/samsung-galaxy-s10-black-back.png</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,8 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,12 +445,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14546F0-777E-F449-8994-801B82B38314}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="38.83203125" customWidth="1"/>
+    <col min="8" max="8" width="40.83203125" customWidth="1"/>
+    <col min="9" max="9" width="70.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>29.79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>29.79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>29.79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Error handling for manager when wrong product details are entered
</commit_message>
<xml_diff>
--- a/static/add_products_template.xlsx
+++ b/static/add_products_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leharbhatt/P9_New_Product_Customizor_App/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF403CA5-CFDE-9E4F-9457-FBEEC8B4F2C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DE09B1-45E5-B940-9FF1-538ADD7DEC43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F36F7B3E-06A3-9447-9F11-6C3B77302C92}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>product_title</t>
   </si>
@@ -47,9 +47,6 @@
     <t>product_category</t>
   </si>
   <si>
-    <t>customizable</t>
-  </si>
-  <si>
     <t>product_image</t>
   </si>
   <si>
@@ -83,10 +80,16 @@
     <t>testing2</t>
   </si>
   <si>
-    <t>testing3</t>
-  </si>
-  <si>
     <t>/Users/leharbhatt/Desktop/samsung-galaxy-s10-black-back.png</t>
+  </si>
+  <si>
+    <t>TestProduct4</t>
+  </si>
+  <si>
+    <t>testing4</t>
+  </si>
+  <si>
+    <t>tesing 3</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14546F0-777E-F449-8994-801B82B38314}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,13 +460,13 @@
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="38.83203125" customWidth="1"/>
-    <col min="8" max="8" width="40.83203125" customWidth="1"/>
-    <col min="9" max="9" width="70.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="38.83203125" customWidth="1"/>
+    <col min="7" max="7" width="40.83203125" customWidth="1"/>
+    <col min="8" max="8" width="70.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,106 +480,120 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
       </c>
       <c r="C2">
         <v>29.79</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>29.79</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>29.79</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
+      <c r="C5">
+        <v>29.79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>